<commit_message>
- Made calculates renderable. - Remove all side-letters other than for 'relevant', 'calculation', and 'choice_filter'. - Removed 'test' template directory.
</commit_message>
<xml_diff>
--- a/test/static/RenderCalculatesInPlace/input/1.xlsx
+++ b/test/static/RenderCalculatesInPlace/input/1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="26500" tabRatio="443"/>
+    <workbookView xWindow="0" yWindow="12800" windowWidth="51200" windowHeight="28260" tabRatio="443"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7507" uniqueCount="2422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7514" uniqueCount="2423">
   <si>
     <t>type</t>
   </si>
@@ -7931,6 +7931,9 @@
   </si>
   <si>
     <t>ppp_excludes</t>
+  </si>
+  <si>
+    <t>Placeholder text for: unlinked</t>
   </si>
 </sst>
 </file>
@@ -8137,7 +8140,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1083">
+  <cellStyleXfs count="1095">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -8959,6 +8962,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -9429,7 +9444,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1083">
+  <cellStyles count="1095">
     <cellStyle name="20% - Accent6" xfId="816" builtinId="50"/>
     <cellStyle name="Excel Built-in Normal" xfId="228"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -9971,6 +9986,12 @@
     <cellStyle name="Followed Hyperlink" xfId="1078" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1080" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1082" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1084" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1086" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1088" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1090" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1092" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1094" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -10510,6 +10531,12 @@
     <cellStyle name="Hyperlink" xfId="1077" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1079" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1081" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1083" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1085" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1087" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1089" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1091" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1093" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="37"/>
     <cellStyle name="Normal 5" xfId="231"/>
@@ -10836,10 +10863,10 @@
   <dimension ref="A1:IW373"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AX2" sqref="AX2"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0"/>
@@ -11056,7 +11083,10 @@
       <c r="B2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="16"/>
+      <c r="C2" s="16" t="str">
+        <f>"Placeholder text for: "&amp;B2</f>
+        <v>Placeholder text for: unlinked</v>
+      </c>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
@@ -12014,7 +12044,10 @@
       <c r="B18" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="16"/>
+      <c r="C18" s="16" t="str">
+        <f>"Placeholder text for: "&amp;B18</f>
+        <v>Placeholder text for: proceed_with_unlinked</v>
+      </c>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
@@ -14086,7 +14119,10 @@
       <c r="B35" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C35" s="16"/>
+      <c r="C35" s="16" t="str">
+        <f>"Placeholder text for: "&amp;B35</f>
+        <v>Placeholder text for: today</v>
+      </c>
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
@@ -15312,6 +15348,10 @@
       <c r="B54" s="36" t="s">
         <v>102</v>
       </c>
+      <c r="C54" s="16" t="str">
+        <f>"Placeholder text for: "&amp;B54</f>
+        <v>Placeholder text for: consent_obtained</v>
+      </c>
       <c r="L54" s="35" t="s">
         <v>2253</v>
       </c>
@@ -15645,7 +15685,10 @@
       <c r="B58" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C58" s="16"/>
+      <c r="C58" s="16" t="str">
+        <f>"Placeholder text for: "&amp;B58</f>
+        <v>Placeholder text for: firstname</v>
+      </c>
       <c r="D58" s="16"/>
       <c r="E58" s="16"/>
       <c r="F58" s="16"/>
@@ -16007,7 +16050,10 @@
       <c r="B65" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="C65" s="53"/>
+      <c r="C65" s="16" t="str">
+        <f>"Placeholder text for: "&amp;B65</f>
+        <v>Placeholder text for: birthdate</v>
+      </c>
       <c r="D65" s="53"/>
       <c r="E65" s="53"/>
       <c r="F65" s="53"/>
@@ -16046,6 +16092,10 @@
       <c r="B67" s="53" t="s">
         <v>2396</v>
       </c>
+      <c r="C67" s="16" t="str">
+        <f>"Placeholder text for: "&amp;B67</f>
+        <v>Placeholder text for: birthday_10yr</v>
+      </c>
       <c r="L67" s="53" t="s">
         <v>2400</v>
       </c>
@@ -16059,7 +16109,10 @@
       <c r="B68" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="C68" s="16"/>
+      <c r="C68" s="16" t="str">
+        <f t="shared" ref="C68:C71" si="0">"Placeholder text for: "&amp;B68</f>
+        <v>Placeholder text for: birthmonth</v>
+      </c>
       <c r="D68" s="16"/>
       <c r="E68" s="16"/>
       <c r="F68" s="16"/>
@@ -16100,7 +16153,10 @@
       <c r="B69" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C69" s="16"/>
+      <c r="C69" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>Placeholder text for: birthyear</v>
+      </c>
       <c r="D69" s="16"/>
       <c r="E69" s="16"/>
       <c r="F69" s="16"/>
@@ -16141,7 +16197,10 @@
       <c r="B70" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="C70" s="16"/>
+      <c r="C70" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>Placeholder text for: thismonth</v>
+      </c>
       <c r="D70" s="16"/>
       <c r="E70" s="16"/>
       <c r="F70" s="16"/>
@@ -16182,7 +16241,10 @@
       <c r="B71" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C71" s="16"/>
+      <c r="C71" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>Placeholder text for: thisyear</v>
+      </c>
       <c r="D71" s="16"/>
       <c r="E71" s="16"/>
       <c r="F71" s="16"/>
@@ -17077,7 +17139,10 @@
       <c r="B86" s="53" t="s">
         <v>141</v>
       </c>
-      <c r="C86" s="53"/>
+      <c r="C86" s="16" t="str">
+        <f>"Placeholder text for: "&amp;B86</f>
+        <v>Placeholder text for: husband_cohabit_start_first</v>
+      </c>
       <c r="D86" s="53"/>
       <c r="E86" s="53"/>
       <c r="F86" s="53"/>
@@ -17132,7 +17197,10 @@
       <c r="B88" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="C88" s="16"/>
+      <c r="C88" s="16" t="str">
+        <f t="shared" ref="C88:C90" si="1">"Placeholder text for: "&amp;B88</f>
+        <v>Placeholder text for: firstmarriagemonth</v>
+      </c>
       <c r="D88" s="16"/>
       <c r="E88" s="16"/>
       <c r="F88" s="16"/>
@@ -17175,7 +17243,10 @@
       <c r="B89" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="C89" s="16"/>
+      <c r="C89" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Placeholder text for: firstmarriageyear</v>
+      </c>
       <c r="D89" s="16"/>
       <c r="E89" s="16"/>
       <c r="F89" s="16"/>
@@ -17218,7 +17289,10 @@
       <c r="B90" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="C90" s="16"/>
+      <c r="C90" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Placeholder text for: young_marriage_first</v>
+      </c>
       <c r="D90" s="16"/>
       <c r="E90" s="16"/>
       <c r="F90" s="16"/>
@@ -17542,6 +17616,10 @@
       <c r="B96" s="54" t="s">
         <v>154</v>
       </c>
+      <c r="C96" s="16" t="str">
+        <f>"Placeholder text for: "&amp;B96</f>
+        <v>Placeholder text for: husband_cohabit_start_recent</v>
+      </c>
       <c r="L96" s="54" t="s">
         <v>2354</v>
       </c>
@@ -17615,7 +17693,10 @@
       <c r="B99" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C99" s="16"/>
+      <c r="C99" s="16" t="str">
+        <f t="shared" ref="C99:C101" si="2">"Placeholder text for: "&amp;B99</f>
+        <v>Placeholder text for: recentmarriagemonth</v>
+      </c>
       <c r="D99" s="16"/>
       <c r="E99" s="16"/>
       <c r="F99" s="16"/>
@@ -17658,7 +17739,10 @@
       <c r="B100" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="C100" s="16"/>
+      <c r="C100" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>Placeholder text for: recentmarriageyear</v>
+      </c>
       <c r="D100" s="16"/>
       <c r="E100" s="16"/>
       <c r="F100" s="16"/>
@@ -17701,7 +17785,10 @@
       <c r="B101" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="C101" s="16"/>
+      <c r="C101" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>Placeholder text for: young_marriage_recent</v>
+      </c>
       <c r="D101" s="16"/>
       <c r="E101" s="16"/>
       <c r="F101" s="16"/>
@@ -19363,7 +19450,10 @@
       <c r="B121" s="10" t="s">
         <v>752</v>
       </c>
-      <c r="C121" s="10"/>
+      <c r="C121" s="16" t="str">
+        <f t="shared" ref="C121:C122" si="3">"Placeholder text for: "&amp;B121</f>
+        <v>Placeholder text for: children_born</v>
+      </c>
       <c r="D121" s="10"/>
       <c r="E121" s="10"/>
       <c r="F121" s="10"/>
@@ -19420,7 +19510,10 @@
       <c r="B122" s="10" t="s">
         <v>1139</v>
       </c>
-      <c r="C122" s="10"/>
+      <c r="C122" s="16" t="str">
+        <f t="shared" si="3"/>
+        <v>Placeholder text for: birth_events</v>
+      </c>
       <c r="D122" s="10"/>
       <c r="E122" s="10"/>
       <c r="F122" s="10"/>
@@ -19861,7 +19954,10 @@
       <c r="B129" s="53" t="s">
         <v>171</v>
       </c>
-      <c r="C129" s="53"/>
+      <c r="C129" s="16" t="str">
+        <f>"Placeholder text for: "&amp;B129</f>
+        <v>Placeholder text for: first_birth</v>
+      </c>
       <c r="D129" s="53"/>
       <c r="E129" s="53"/>
       <c r="F129" s="53"/>
@@ -20126,7 +20222,10 @@
       <c r="B135" s="53" t="s">
         <v>173</v>
       </c>
-      <c r="C135" s="53"/>
+      <c r="C135" s="16" t="str">
+        <f>"Placeholder text for: "&amp;B135</f>
+        <v>Placeholder text for: recent_birth</v>
+      </c>
       <c r="D135" s="53"/>
       <c r="E135" s="53"/>
       <c r="F135" s="53"/>
@@ -20457,7 +20556,10 @@
       <c r="B143" s="53" t="s">
         <v>175</v>
       </c>
-      <c r="C143" s="53"/>
+      <c r="C143" s="16" t="str">
+        <f>"Placeholder text for: "&amp;B143</f>
+        <v>Placeholder text for: penultimate_birth</v>
+      </c>
       <c r="D143" s="53"/>
       <c r="E143" s="53"/>
       <c r="F143" s="53"/>
@@ -20890,7 +20992,10 @@
       <c r="B153" s="53" t="s">
         <v>178</v>
       </c>
-      <c r="C153" s="53"/>
+      <c r="C153" s="16" t="str">
+        <f>"Placeholder text for: "&amp;B153</f>
+        <v>Placeholder text for: child_death</v>
+      </c>
       <c r="D153" s="53"/>
       <c r="E153" s="53"/>
       <c r="F153" s="53"/>
@@ -21106,7 +21211,10 @@
       <c r="B158" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="C158" s="16"/>
+      <c r="C158" s="16" t="str">
+        <f>"Placeholder text for: "&amp;B158</f>
+        <v>Placeholder text for: menstrual_period_lab</v>
+      </c>
       <c r="D158" s="16"/>
       <c r="E158" s="16"/>
       <c r="F158" s="16"/>
@@ -21561,7 +21669,10 @@
       <c r="B163" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="C163" s="16"/>
+      <c r="C163" s="16" t="str">
+        <f t="shared" ref="C163:C164" si="4">"Placeholder text for: "&amp;B163</f>
+        <v>Placeholder text for: month_calculation</v>
+      </c>
       <c r="D163" s="16"/>
       <c r="E163" s="16"/>
       <c r="F163" s="16"/>
@@ -21604,7 +21715,10 @@
       <c r="B164" s="16" t="s">
         <v>766</v>
       </c>
-      <c r="C164" s="16"/>
+      <c r="C164" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>Placeholder text for: rec_birth_date</v>
+      </c>
       <c r="D164" s="16"/>
       <c r="E164" s="16"/>
       <c r="F164" s="16"/>
@@ -22663,7 +22777,10 @@
       <c r="B178" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="C178" s="16"/>
+      <c r="C178" s="16" t="str">
+        <f>"Placeholder text for: "&amp;B178</f>
+        <v>Placeholder text for: waitchild</v>
+      </c>
       <c r="D178" s="16"/>
       <c r="E178" s="16"/>
       <c r="F178" s="16"/>
@@ -25815,7 +25932,10 @@
       <c r="B221" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="C221" s="10"/>
+      <c r="C221" s="16" t="str">
+        <f t="shared" ref="C221:C223" si="5">"Placeholder text for: "&amp;B221</f>
+        <v>Placeholder text for: current_or_recent_user</v>
+      </c>
       <c r="D221" s="10"/>
       <c r="E221" s="10"/>
       <c r="F221" s="10"/>
@@ -25872,7 +25992,10 @@
       <c r="B222" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="C222" s="10"/>
+      <c r="C222" s="16" t="str">
+        <f t="shared" si="5"/>
+        <v>Placeholder text for: current_recent_method</v>
+      </c>
       <c r="D222" s="10"/>
       <c r="E222" s="10"/>
       <c r="F222" s="10"/>
@@ -25929,7 +26052,10 @@
       <c r="B223" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="C223" s="10"/>
+      <c r="C223" s="16" t="str">
+        <f t="shared" si="5"/>
+        <v>Placeholder text for: current_recent_label</v>
+      </c>
       <c r="D223" s="10"/>
       <c r="E223" s="10"/>
       <c r="F223" s="10"/>
@@ -26140,6 +26266,10 @@
       <c r="B226" s="16" t="s">
         <v>834</v>
       </c>
+      <c r="C226" s="16" t="str">
+        <f>"Placeholder text for: "&amp;B226</f>
+        <v>Placeholder text for: rec_husband_date</v>
+      </c>
       <c r="L226" s="16" t="s">
         <v>835</v>
       </c>
@@ -26486,7 +26616,10 @@
       <c r="B233" s="53" t="s">
         <v>266</v>
       </c>
-      <c r="C233" s="53"/>
+      <c r="C233" s="16" t="str">
+        <f>"Placeholder text for: "&amp;B233</f>
+        <v>Placeholder text for: begin_using</v>
+      </c>
       <c r="D233" s="53"/>
       <c r="E233" s="53"/>
       <c r="F233" s="53"/>
@@ -26820,7 +26953,10 @@
       <c r="B241" s="53" t="s">
         <v>268</v>
       </c>
-      <c r="C241" s="53"/>
+      <c r="C241" s="16" t="str">
+        <f>"Placeholder text for: "&amp;B241</f>
+        <v>Placeholder text for: stop_using</v>
+      </c>
       <c r="D241" s="53"/>
       <c r="E241" s="53"/>
       <c r="F241" s="53"/>
@@ -27224,7 +27360,10 @@
       <c r="B250" s="53" t="s">
         <v>866</v>
       </c>
-      <c r="C250" s="53"/>
+      <c r="C250" s="16" t="str">
+        <f>"Placeholder text for: "&amp;B250</f>
+        <v>Placeholder text for: ante_start_using</v>
+      </c>
       <c r="D250" s="53"/>
       <c r="E250" s="53"/>
       <c r="F250" s="53"/>
@@ -27326,7 +27465,10 @@
       <c r="B254" s="16" t="s">
         <v>867</v>
       </c>
-      <c r="C254" s="16"/>
+      <c r="C254" s="16" t="str">
+        <f t="shared" ref="C254:C255" si="6">"Placeholder text for: "&amp;B254</f>
+        <v>Placeholder text for: ante_start_using_m_y</v>
+      </c>
       <c r="D254" s="16"/>
       <c r="E254" s="16"/>
       <c r="F254" s="16"/>
@@ -27368,7 +27510,10 @@
       <c r="B255" s="16" t="s">
         <v>869</v>
       </c>
-      <c r="C255" s="16"/>
+      <c r="C255" s="16" t="str">
+        <f t="shared" si="6"/>
+        <v>Placeholder text for: stop_using_m_y</v>
+      </c>
       <c r="D255" s="16"/>
       <c r="E255" s="16"/>
       <c r="F255" s="16"/>
@@ -27689,7 +27834,10 @@
       <c r="B260" s="16" t="s">
         <v>273</v>
       </c>
-      <c r="C260" s="16"/>
+      <c r="C260" s="16" t="str">
+        <f t="shared" ref="C260:C262" si="7">"Placeholder text for: "&amp;B260</f>
+        <v>Placeholder text for: begin_using_lab</v>
+      </c>
       <c r="D260" s="16"/>
       <c r="E260" s="16"/>
       <c r="F260" s="16"/>
@@ -27731,7 +27879,10 @@
       <c r="B261" s="16" t="s">
         <v>879</v>
       </c>
-      <c r="C261" s="16"/>
+      <c r="C261" s="16" t="str">
+        <f t="shared" si="7"/>
+        <v>Placeholder text for: ante_start_lab</v>
+      </c>
       <c r="D261" s="16"/>
       <c r="E261" s="16"/>
       <c r="F261" s="16"/>
@@ -27773,7 +27924,10 @@
       <c r="B262" s="16" t="s">
         <v>1089</v>
       </c>
-      <c r="C262" s="16"/>
+      <c r="C262" s="16" t="str">
+        <f t="shared" si="7"/>
+        <v>Placeholder text for: start_date_lab</v>
+      </c>
       <c r="D262" s="16"/>
       <c r="E262" s="16"/>
       <c r="F262" s="16"/>
@@ -28928,7 +29082,10 @@
       <c r="B278" s="10" t="s">
         <v>901</v>
       </c>
-      <c r="C278" s="10"/>
+      <c r="C278" s="16" t="str">
+        <f>"Placeholder text for: "&amp;B278</f>
+        <v>Placeholder text for: provider_label</v>
+      </c>
       <c r="D278" s="10"/>
       <c r="E278" s="10"/>
       <c r="F278" s="10"/>
@@ -29377,7 +29534,10 @@
       <c r="B284" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="C284" s="16"/>
+      <c r="C284" s="16" t="str">
+        <f t="shared" ref="C284:C285" si="8">"Placeholder text for: "&amp;B284</f>
+        <v>Placeholder text for: fp_ever_used</v>
+      </c>
       <c r="D284" s="16"/>
       <c r="E284" s="16"/>
       <c r="F284" s="16"/>
@@ -29419,7 +29579,10 @@
       <c r="B285" s="16" t="s">
         <v>1010</v>
       </c>
-      <c r="C285" s="16"/>
+      <c r="C285" s="16" t="str">
+        <f t="shared" si="8"/>
+        <v>Placeholder text for: age_begin_using</v>
+      </c>
       <c r="D285" s="16"/>
       <c r="E285" s="16"/>
       <c r="F285" s="16"/>
@@ -31825,7 +31988,9 @@
       <c r="B318" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="C318" s="61"/>
+      <c r="C318" s="31" t="s">
+        <v>2422</v>
+      </c>
       <c r="D318" s="16"/>
       <c r="E318" s="16"/>
       <c r="F318" s="16"/>
@@ -32442,7 +32607,9 @@
       <c r="B327" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="C327" s="16"/>
+      <c r="C327" s="31" t="s">
+        <v>2422</v>
+      </c>
       <c r="D327" s="16"/>
       <c r="E327" s="16"/>
       <c r="F327" s="16"/>
@@ -32830,7 +32997,9 @@
       <c r="B331" s="16" t="s">
         <v>344</v>
       </c>
-      <c r="C331" s="16"/>
+      <c r="C331" s="31" t="s">
+        <v>2422</v>
+      </c>
       <c r="D331" s="16"/>
       <c r="E331" s="16"/>
       <c r="F331" s="16"/>
@@ -33266,6 +33435,9 @@
       <c r="B338" s="10" t="s">
         <v>351</v>
       </c>
+      <c r="C338" s="31" t="s">
+        <v>2422</v>
+      </c>
       <c r="L338" s="10" t="s">
         <v>352</v>
       </c>
@@ -33935,6 +34107,9 @@
       <c r="B348" s="10" t="s">
         <v>1045</v>
       </c>
+      <c r="C348" s="31" t="s">
+        <v>2422</v>
+      </c>
       <c r="L348" s="10" t="s">
         <v>1046</v>
       </c>
@@ -34042,6 +34217,9 @@
       <c r="B350" s="10" t="s">
         <v>1051</v>
       </c>
+      <c r="C350" s="31" t="s">
+        <v>2422</v>
+      </c>
       <c r="L350" s="19" t="s">
         <v>1052</v>
       </c>
@@ -34360,6 +34538,9 @@
       </c>
       <c r="B355" s="10" t="s">
         <v>1066</v>
+      </c>
+      <c r="C355" s="31" t="s">
+        <v>2422</v>
       </c>
       <c r="L355" s="10" t="s">
         <v>1067</v>

</xml_diff>